<commit_message>
tambah fitur cetak cepat
</commit_message>
<xml_diff>
--- a/public/file_alumni_excel/contoh/Contoh.xlsx
+++ b/public/file_alumni_excel/contoh/Contoh.xlsx
@@ -1,48 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SID\Desktop\New folder (4)\SistemInformasiAlumni\public\file_alumni_excel\contoh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SID\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DA3AC2-208A-4449-B2C5-651997521A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0614621-32F6-46FA-8E1E-41B41F6E0455}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{FB25568F-381E-4287-B9FD-2BFF8C52D038}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tets" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Nama Alumni</t>
+    <t>subhan assiddik</t>
   </si>
   <si>
-    <t>Nim</t>
-  </si>
-  <si>
-    <t>Alamat Email</t>
-  </si>
-  <si>
-    <t>No Telepon</t>
+    <t>subhanassiddik@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -87,9 +75,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -126,7 +113,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -138,7 +125,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -185,23 +172,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -237,23 +207,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -405,51 +358,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5762C006-0E68-4380-BDFA-6DA6BC684DAE}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1">
+        <v>201721021</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+      <c r="D1">
+        <v>85256199655</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="subhanassiddik@gmail.com" xr:uid="{27C0D969-542B-4DA7-AFC9-D37F716209D8}"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{0485F10F-554F-4187-8E46-558A904D6CE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>